<commit_message>
completed draft 1 cond-valid
</commit_message>
<xml_diff>
--- a/BIS232_CONDITION_VALIDATION/input_data/datapool/Exclusion_Conditions_2.xlsx
+++ b/BIS232_CONDITION_VALIDATION/input_data/datapool/Exclusion_Conditions_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mouloud Hamdidouche\Desktop\eclipse\SeleniumProjects\BIS232_CONDITION_VALIDATION\input_data\datapool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50FE6AD4-458C-46EE-A5BD-15CACEF62D58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F101BCFF-B698-4C0A-B302-875A37210E5B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19776" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69378,8 +69378,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>